<commit_message>
committing order detail page,credit and advance page and confirm order page changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\eclipse-workspace\DCPLProject\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E64924-9558-4406-8984-DD5E6D33C69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823BDAAB-A564-4A4B-940C-9EB157694659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="106">
   <si>
     <t>hrms_id</t>
   </si>
@@ -242,13 +242,118 @@
   </si>
   <si>
     <t>98</t>
+  </si>
+  <si>
+    <t>orderKind</t>
+  </si>
+  <si>
+    <t>New Order-NO</t>
+  </si>
+  <si>
+    <t>segmentType</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>jewelType</t>
+  </si>
+  <si>
+    <t>Necklace</t>
+  </si>
+  <si>
+    <t>Pieces</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>vendorCode</t>
+  </si>
+  <si>
+    <t>BKK</t>
+  </si>
+  <si>
+    <t>mainCategory</t>
+  </si>
+  <si>
+    <t>subCategory</t>
+  </si>
+  <si>
+    <t>dueDateMonth</t>
+  </si>
+  <si>
+    <t>dueDateYear</t>
+  </si>
+  <si>
+    <t>dueDateDay</t>
+  </si>
+  <si>
+    <t>salesExecutiveID</t>
+  </si>
+  <si>
+    <t>metalColor</t>
+  </si>
+  <si>
+    <t>skinPurity</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>metalWeightType</t>
+  </si>
+  <si>
+    <t>fromWeightRange</t>
+  </si>
+  <si>
+    <t>toWeightRange</t>
+  </si>
+  <si>
+    <t>expectedWeightRange</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>lengthSearch</t>
+  </si>
+  <si>
+    <t>7.5"</t>
+  </si>
+  <si>
+    <t>hookTypeSearch</t>
+  </si>
+  <si>
+    <t>U Hook</t>
+  </si>
+  <si>
+    <t>polishTypeSearch</t>
+  </si>
+  <si>
+    <t>settingTypeSearch</t>
+  </si>
+  <si>
+    <t>Matt Finish</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Open Setting</t>
+  </si>
+  <si>
+    <t>payAdvOption</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +384,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -300,7 +411,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -360,12 +471,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -379,6 +514,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1005,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C652DA7-46DF-4FCD-BBC9-BFF7179281CD}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1088,9 +1227,7 @@
       <c r="E2" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>51</v>
-      </c>
+      <c r="F2" s="7"/>
       <c r="G2" s="12" t="s">
         <v>62</v>
       </c>
@@ -1130,15 +1267,33 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D04161-DFF8-4095-A5EB-FA021B973EF1}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1184,8 +1339,74 @@
       <c r="O1" s="11" t="s">
         <v>61</v>
       </c>
+      <c r="P1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC1" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG1" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>70</v>
       </c>
@@ -1201,9 +1422,7 @@
       <c r="E2" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>51</v>
-      </c>
+      <c r="F2" s="7"/>
       <c r="G2" s="12" t="s">
         <v>62</v>
       </c>
@@ -1214,7 +1433,7 @@
         <v>64</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>66</v>
@@ -1229,6 +1448,72 @@
         <v>69</v>
       </c>
       <c r="O2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="W2" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z2" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA2" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB2" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD2" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE2" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF2" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="AG2" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="AH2" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI2" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="AJ2" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AK2" s="4" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1237,5 +1522,6 @@
     <hyperlink ref="B2" r:id="rId1" xr:uid="{BBF7843D-139F-41D2-B6CA-9C7C631E7590}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commiting pom.xml and test data excel changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\eclipse-workspace\DCPLProject\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823BDAAB-A564-4A4B-940C-9EB157694659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1E2F5E-B416-4BFC-A87D-87BF8EF36BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="108">
   <si>
     <t>hrms_id</t>
   </si>
@@ -241,9 +241,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>98</t>
-  </si>
-  <si>
     <t>orderKind</t>
   </si>
   <si>
@@ -347,6 +344,15 @@
   </si>
   <si>
     <t>payAdvOption</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
@@ -817,7 +823,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -836,7 +842,7 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -936,7 +942,7 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -1053,7 +1059,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -1073,7 +1079,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -1087,7 +1093,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -1101,7 +1107,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
@@ -1115,7 +1121,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
@@ -1144,8 +1150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C652DA7-46DF-4FCD-BBC9-BFF7179281CD}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:J2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1213,7 +1219,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
@@ -1232,7 +1238,7 @@
         <v>62</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>64</v>
@@ -1269,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D04161-DFF8-4095-A5EB-FA021B973EF1}">
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1340,75 +1346,75 @@
         <v>61</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="U1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="V1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="AA1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="AB1" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="AC1" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="AF1" s="3" t="s">
-        <v>93</v>
-      </c>
       <c r="AG1" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AH1" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AI1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AJ1" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="AK1" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
@@ -1427,13 +1433,13 @@
         <v>62</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>64</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>66</v>
@@ -1451,25 +1457,25 @@
         <v>67</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R2" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="W2" s="12" t="s">
         <v>63</v>
@@ -1478,40 +1484,40 @@
         <v>64</v>
       </c>
       <c r="Y2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z2" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA2" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB2" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD2" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE2" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF2" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG2" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="AH2" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AJ2" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="Z2" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="AA2" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB2" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="AD2" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="AE2" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AF2" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AG2" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="AH2" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI2" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="AJ2" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="AK2" s="4" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
this is my latest commit on 31-01-23
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\eclipse-workspace\DCPLProject\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1E2F5E-B416-4BFC-A87D-87BF8EF36BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE7FCB3-070D-4276-87B3-C4EB2198A9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SalesLogin" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,10 @@
     <sheet name="SearchCustomerDetails" sheetId="4" r:id="rId3"/>
     <sheet name="OrderHeaderPage" sheetId="5" r:id="rId4"/>
     <sheet name="OrderDetailPage" sheetId="6" r:id="rId5"/>
+    <sheet name="OrderConfirmationPage" sheetId="8" r:id="rId6"/>
+    <sheet name="CashierReceipts" sheetId="9" r:id="rId7"/>
+    <sheet name="StoreHeadConfirmationPage" sheetId="12" r:id="rId8"/>
+    <sheet name="CreateCustomerOrderNo" sheetId="14" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="176">
   <si>
     <t>hrms_id</t>
   </si>
@@ -220,9 +224,6 @@
     <t>Self</t>
   </si>
   <si>
-    <t>Nov</t>
-  </si>
-  <si>
     <t>2022</t>
   </si>
   <si>
@@ -337,9 +338,6 @@
     <t>Matt Finish</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>Open Setting</t>
   </si>
   <si>
@@ -352,7 +350,217 @@
     <t>Dec</t>
   </si>
   <si>
-    <t>10</t>
+    <t>payAdvAmount</t>
+  </si>
+  <si>
+    <t>25000.00</t>
+  </si>
+  <si>
+    <t>CashAmount</t>
+  </si>
+  <si>
+    <t>payModesOption2</t>
+  </si>
+  <si>
+    <t>payModesOption1</t>
+  </si>
+  <si>
+    <t>MultipleMode</t>
+  </si>
+  <si>
+    <t>ChequeDD</t>
+  </si>
+  <si>
+    <t>chequeDDType</t>
+  </si>
+  <si>
+    <t>accHolderName</t>
+  </si>
+  <si>
+    <t>accNumber</t>
+  </si>
+  <si>
+    <t>chequeNumber</t>
+  </si>
+  <si>
+    <t>cheque</t>
+  </si>
+  <si>
+    <t>Hashmi</t>
+  </si>
+  <si>
+    <t>5263415296857485</t>
+  </si>
+  <si>
+    <t>415263</t>
+  </si>
+  <si>
+    <t>chequeMonth</t>
+  </si>
+  <si>
+    <t>chequeYear</t>
+  </si>
+  <si>
+    <t>chequeDay</t>
+  </si>
+  <si>
+    <t>bankName</t>
+  </si>
+  <si>
+    <t>branchName</t>
+  </si>
+  <si>
+    <t>Banshankari</t>
+  </si>
+  <si>
+    <t>chequeAmount</t>
+  </si>
+  <si>
+    <t>Axis Bank</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>cardNumber</t>
+  </si>
+  <si>
+    <t>4152639685</t>
+  </si>
+  <si>
+    <t>cardType</t>
+  </si>
+  <si>
+    <t>RUPAY</t>
+  </si>
+  <si>
+    <t>nameOnCard</t>
+  </si>
+  <si>
+    <t>cardExpiryMonth</t>
+  </si>
+  <si>
+    <t>cardExpiryYear</t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
+  <si>
+    <t>cardBankName</t>
+  </si>
+  <si>
+    <t>cardBank</t>
+  </si>
+  <si>
+    <t>AXIS</t>
+  </si>
+  <si>
+    <t>authID</t>
+  </si>
+  <si>
+    <t>41526</t>
+  </si>
+  <si>
+    <t>cardAmount</t>
+  </si>
+  <si>
+    <t>Debit Card</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>adjustType</t>
+  </si>
+  <si>
+    <t>adjustmentAmount</t>
+  </si>
+  <si>
+    <t>1000.00</t>
+  </si>
+  <si>
+    <t>adjustmentNumber</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Payment Voucher</t>
+  </si>
+  <si>
+    <t>firstGiftVoucherNumber</t>
+  </si>
+  <si>
+    <t>secondGiftVoucherNumber</t>
+  </si>
+  <si>
+    <t>noOfGiftVouchers</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>5000.00</t>
+  </si>
+  <si>
+    <t>frommonth</t>
+  </si>
+  <si>
+    <t>fromyear</t>
+  </si>
+  <si>
+    <t>fromday</t>
+  </si>
+  <si>
+    <t>tomonth</t>
+  </si>
+  <si>
+    <t>toyear</t>
+  </si>
+  <si>
+    <t>today</t>
+  </si>
+  <si>
+    <t>orderno</t>
+  </si>
+  <si>
+    <t>salesexecutive</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>orderstatus</t>
+  </si>
+  <si>
+    <t>Ready</t>
+  </si>
+  <si>
+    <t>cashierhrms_id</t>
+  </si>
+  <si>
+    <t>cashierpassword</t>
+  </si>
+  <si>
+    <t>31</t>
   </si>
 </sst>
 </file>
@@ -506,7 +714,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -519,11 +727,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -823,7 +1039,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -942,7 +1158,7 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -1059,7 +1275,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -1079,7 +1295,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -1093,7 +1309,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -1107,7 +1323,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
@@ -1121,7 +1337,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
@@ -1219,7 +1435,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
@@ -1234,32 +1450,32 @@
         <v>52</v>
       </c>
       <c r="F2" s="7"/>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>106</v>
+      <c r="H2" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="M2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="N2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="O2" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1273,10 +1489,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D04161-DFF8-4095-A5EB-FA021B973EF1}">
-  <dimension ref="A1:AK2"/>
+  <dimension ref="A1:BP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView topLeftCell="BD1" workbookViewId="0">
+      <selection sqref="A1:BP2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1297,9 +1513,34 @@
     <col min="35" max="35" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.44140625" customWidth="1"/>
+    <col min="40" max="40" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="19.6640625" customWidth="1"/>
+    <col min="42" max="42" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="46" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="14" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="18" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="66" max="67" width="18" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1346,75 +1587,168 @@
         <v>61</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="U1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="V1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="AA1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="AB1" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC1" s="15" t="s">
+      <c r="AC1" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="AF1" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="AG1" s="13" t="s">
-        <v>95</v>
+      <c r="AG1" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="AH1" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AI1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="AJ1" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="AK1" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AM1" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="AN1" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="AO1" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AQ1" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="AR1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS1" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="AT1" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="AU1" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV1" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="AW1" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="AX1" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="AY1" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="AZ1" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="BA1" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="BB1" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="BC1" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="BD1" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="BE1" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF1" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="BG1" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="BH1" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="BI1" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="BJ1" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="BK1" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="BL1" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="BM1" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="BN1" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="BO1" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="BP1" s="16" t="s">
+        <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
@@ -1429,98 +1763,191 @@
         <v>52</v>
       </c>
       <c r="F2" s="7"/>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="Z2" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE2" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF2" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="AG2" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="AH2" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL2" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="AM2" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN2" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="AO2" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AP2" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AR2" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS2" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="AT2" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AV2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AZ2" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="BA2" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="BC2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="BE2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="BF2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="BG2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="BH2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="BI2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q2" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="R2" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="Z2" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="AA2" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB2" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="AD2" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="AE2" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="AF2" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="AG2" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="AH2" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="AI2" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="AJ2" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="AK2" s="4" t="s">
-        <v>67</v>
+      <c r="BK2" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="BL2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="BM2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="BN2" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="BO2" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="BP2" s="2" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1530,4 +1957,638 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CDBC5E9-01B9-4A17-8E18-82575898BD8D}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{129DB296-04C0-4141-B533-E5D5D6FBB2BF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51FBBC2E-A265-495D-AA22-AE60D0509044}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{75FF7960-2D4A-4F48-9082-5E5A6ACEBC07}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC6B23FB-F06E-4C7D-A14C-C7F88539098D}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{548A1AC8-7B92-4E61-9570-922F94BF4D27}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D83E6DB-5A04-4CE4-AB6C-9127F09B31CE}">
+  <dimension ref="A1:BP2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="57" max="57" width="17.88671875" customWidth="1"/>
+    <col min="68" max="68" width="24.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:68" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z1" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC1" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AG1" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AM1" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="AN1" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="AO1" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AQ1" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="AR1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS1" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="AT1" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="AU1" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV1" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="AW1" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="AX1" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="AY1" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="AZ1" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="BA1" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="BB1" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="BC1" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="BD1" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="BE1" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF1" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="BG1" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="BH1" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="BI1" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="BJ1" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="BK1" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="BL1" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="BM1" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="BN1" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="BO1" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="BP1" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:68" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="Z2" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE2" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF2" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="AG2" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="AH2" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL2" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="AM2" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN2" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="AO2" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AP2" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AR2" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS2" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="AT2" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AV2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AZ2" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="BA2" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="BC2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="BE2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="BF2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="BG2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="BH2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="BI2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="BK2" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="BL2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="BM2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="BN2" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="BO2" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="BP2" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{C5D462F1-3D8C-4C77-9D09-C81D13C3EE40}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated test data excel
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\eclipse-workspace\DCPLProject\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE7FCB3-070D-4276-87B3-C4EB2198A9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9D56A8-928C-4BE2-BF41-A5574B770672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="177">
   <si>
     <t>hrms_id</t>
   </si>
@@ -560,7 +560,10 @@
     <t>cashierpassword</t>
   </si>
   <si>
-    <t>31</t>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>28</t>
   </si>
 </sst>
 </file>
@@ -1367,7 +1370,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1491,8 +1494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D04161-DFF8-4095-A5EB-FA021B973EF1}">
   <dimension ref="A1:BP2"/>
   <sheetViews>
-    <sheetView topLeftCell="BD1" workbookViewId="0">
-      <selection sqref="A1:BP2"/>
+    <sheetView topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AM2" sqref="AM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1964,7 +1967,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2009,22 +2012,22 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>128</v>
+        <v>175</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>129</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>175</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>129</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>175</v>
+        <v>76</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
@@ -2128,22 +2131,22 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>128</v>
+        <v>175</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>129</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>175</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>129</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>175</v>
+        <v>76</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
@@ -2402,13 +2405,13 @@
         <v>62</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>128</v>
+        <v>175</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>129</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>65</v>
@@ -2447,13 +2450,13 @@
         <v>76</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>128</v>
+        <v>175</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>129</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="Z2" s="13" t="s">
         <v>87</v>
@@ -2519,13 +2522,13 @@
         <v>119</v>
       </c>
       <c r="AU2" s="2" t="s">
-        <v>128</v>
+        <v>175</v>
       </c>
       <c r="AV2" s="2" t="s">
         <v>129</v>
       </c>
       <c r="AW2" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AX2" s="2" t="s">
         <v>127</v>

</xml_diff>